<commit_message>
added 45C data from USDA and updated size scaling
</commit_message>
<xml_diff>
--- a/data/thermal-curve/metadata.xlsx
+++ b/data/thermal-curve/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-assay-development/data/thermal-curve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A672A69-BAA4-2F42-8C8B-C8C9BB9771D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951ACFA3-1685-E84D-8F1A-16277CD9573B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19020" yWindow="760" windowWidth="10540" windowHeight="17760" xr2:uid="{6EE03324-2EC3-1948-92E0-D75DA66F4FFC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="40">
   <si>
     <t>A01</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>plate2</t>
+  </si>
+  <si>
+    <t>C06</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5943EADD-18D6-C34A-B3B5-063A7A4D8310}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3023,6 +3026,516 @@
         <v>30</v>
       </c>
     </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>20250820</v>
+      </c>
+      <c r="B147" t="s">
+        <v>37</v>
+      </c>
+      <c r="C147">
+        <v>45</v>
+      </c>
+      <c r="D147" t="s">
+        <v>0</v>
+      </c>
+      <c r="E147" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>20250820</v>
+      </c>
+      <c r="B148" t="s">
+        <v>37</v>
+      </c>
+      <c r="C148">
+        <v>45</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1</v>
+      </c>
+      <c r="E148" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>20250820</v>
+      </c>
+      <c r="B149" t="s">
+        <v>37</v>
+      </c>
+      <c r="C149">
+        <v>45</v>
+      </c>
+      <c r="D149" t="s">
+        <v>2</v>
+      </c>
+      <c r="E149" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>20250820</v>
+      </c>
+      <c r="B150" t="s">
+        <v>37</v>
+      </c>
+      <c r="C150">
+        <v>45</v>
+      </c>
+      <c r="D150" t="s">
+        <v>3</v>
+      </c>
+      <c r="E150" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>20250820</v>
+      </c>
+      <c r="B151" t="s">
+        <v>37</v>
+      </c>
+      <c r="C151">
+        <v>45</v>
+      </c>
+      <c r="D151" t="s">
+        <v>12</v>
+      </c>
+      <c r="E151" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>20250820</v>
+      </c>
+      <c r="B152" t="s">
+        <v>37</v>
+      </c>
+      <c r="C152">
+        <v>45</v>
+      </c>
+      <c r="D152" t="s">
+        <v>13</v>
+      </c>
+      <c r="E152" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>20250820</v>
+      </c>
+      <c r="B153" t="s">
+        <v>37</v>
+      </c>
+      <c r="C153">
+        <v>45</v>
+      </c>
+      <c r="D153" t="s">
+        <v>14</v>
+      </c>
+      <c r="E153" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>20250820</v>
+      </c>
+      <c r="B154" t="s">
+        <v>37</v>
+      </c>
+      <c r="C154">
+        <v>45</v>
+      </c>
+      <c r="D154" t="s">
+        <v>15</v>
+      </c>
+      <c r="E154" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>20250820</v>
+      </c>
+      <c r="B155" t="s">
+        <v>37</v>
+      </c>
+      <c r="C155">
+        <v>45</v>
+      </c>
+      <c r="D155" t="s">
+        <v>16</v>
+      </c>
+      <c r="E155" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>20250820</v>
+      </c>
+      <c r="B156" t="s">
+        <v>37</v>
+      </c>
+      <c r="C156">
+        <v>45</v>
+      </c>
+      <c r="D156" t="s">
+        <v>17</v>
+      </c>
+      <c r="E156" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>20250820</v>
+      </c>
+      <c r="B157" t="s">
+        <v>37</v>
+      </c>
+      <c r="C157">
+        <v>45</v>
+      </c>
+      <c r="D157" t="s">
+        <v>18</v>
+      </c>
+      <c r="E157" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>20250820</v>
+      </c>
+      <c r="B158" t="s">
+        <v>37</v>
+      </c>
+      <c r="C158">
+        <v>45</v>
+      </c>
+      <c r="D158" t="s">
+        <v>19</v>
+      </c>
+      <c r="E158" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>20250820</v>
+      </c>
+      <c r="B159" t="s">
+        <v>37</v>
+      </c>
+      <c r="C159">
+        <v>45</v>
+      </c>
+      <c r="D159" t="s">
+        <v>4</v>
+      </c>
+      <c r="E159" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>20250820</v>
+      </c>
+      <c r="B160" t="s">
+        <v>37</v>
+      </c>
+      <c r="C160">
+        <v>45</v>
+      </c>
+      <c r="D160" t="s">
+        <v>5</v>
+      </c>
+      <c r="E160" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>20250820</v>
+      </c>
+      <c r="B161" t="s">
+        <v>37</v>
+      </c>
+      <c r="C161">
+        <v>45</v>
+      </c>
+      <c r="D161" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>20250820</v>
+      </c>
+      <c r="B162" t="s">
+        <v>37</v>
+      </c>
+      <c r="C162">
+        <v>45</v>
+      </c>
+      <c r="D162" t="s">
+        <v>7</v>
+      </c>
+      <c r="E162" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>20250820</v>
+      </c>
+      <c r="B163" t="s">
+        <v>37</v>
+      </c>
+      <c r="C163">
+        <v>45</v>
+      </c>
+      <c r="D163" t="s">
+        <v>20</v>
+      </c>
+      <c r="E163" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>20250820</v>
+      </c>
+      <c r="B164" t="s">
+        <v>37</v>
+      </c>
+      <c r="C164">
+        <v>45</v>
+      </c>
+      <c r="D164" t="s">
+        <v>21</v>
+      </c>
+      <c r="E164" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>20250820</v>
+      </c>
+      <c r="B165" t="s">
+        <v>37</v>
+      </c>
+      <c r="C165">
+        <v>45</v>
+      </c>
+      <c r="D165" t="s">
+        <v>22</v>
+      </c>
+      <c r="E165" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>20250820</v>
+      </c>
+      <c r="B166" t="s">
+        <v>37</v>
+      </c>
+      <c r="C166">
+        <v>45</v>
+      </c>
+      <c r="D166" t="s">
+        <v>23</v>
+      </c>
+      <c r="E166" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>20250820</v>
+      </c>
+      <c r="B167" t="s">
+        <v>37</v>
+      </c>
+      <c r="C167">
+        <v>45</v>
+      </c>
+      <c r="D167" t="s">
+        <v>24</v>
+      </c>
+      <c r="E167" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>20250820</v>
+      </c>
+      <c r="B168" t="s">
+        <v>37</v>
+      </c>
+      <c r="C168">
+        <v>45</v>
+      </c>
+      <c r="D168" t="s">
+        <v>25</v>
+      </c>
+      <c r="E168" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>20250820</v>
+      </c>
+      <c r="B169" t="s">
+        <v>37</v>
+      </c>
+      <c r="C169">
+        <v>45</v>
+      </c>
+      <c r="D169" t="s">
+        <v>26</v>
+      </c>
+      <c r="E169" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>20250820</v>
+      </c>
+      <c r="B170" t="s">
+        <v>37</v>
+      </c>
+      <c r="C170">
+        <v>45</v>
+      </c>
+      <c r="D170" t="s">
+        <v>27</v>
+      </c>
+      <c r="E170" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>20250820</v>
+      </c>
+      <c r="B171" t="s">
+        <v>37</v>
+      </c>
+      <c r="C171">
+        <v>45</v>
+      </c>
+      <c r="D171" t="s">
+        <v>8</v>
+      </c>
+      <c r="E171" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>20250820</v>
+      </c>
+      <c r="B172" t="s">
+        <v>37</v>
+      </c>
+      <c r="C172">
+        <v>45</v>
+      </c>
+      <c r="D172" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>20250820</v>
+      </c>
+      <c r="B173" t="s">
+        <v>37</v>
+      </c>
+      <c r="C173">
+        <v>45</v>
+      </c>
+      <c r="D173" t="s">
+        <v>10</v>
+      </c>
+      <c r="E173" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>20250820</v>
+      </c>
+      <c r="B174" t="s">
+        <v>37</v>
+      </c>
+      <c r="C174">
+        <v>45</v>
+      </c>
+      <c r="D174" t="s">
+        <v>11</v>
+      </c>
+      <c r="E174" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>20250820</v>
+      </c>
+      <c r="B175" t="s">
+        <v>37</v>
+      </c>
+      <c r="C175">
+        <v>45</v>
+      </c>
+      <c r="D175" t="s">
+        <v>28</v>
+      </c>
+      <c r="E175" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>20250820</v>
+      </c>
+      <c r="B176" t="s">
+        <v>37</v>
+      </c>
+      <c r="C176">
+        <v>45</v>
+      </c>
+      <c r="D176" t="s">
+        <v>39</v>
+      </c>
+      <c r="E176" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>